<commit_message>
add presentation deck and update readme file with the link to the presentation deck - revision 2
</commit_message>
<xml_diff>
--- a/Final-PBI_Ordered_List.xlsx
+++ b/Final-PBI_Ordered_List.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="18195" windowHeight="7230"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="28220" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="209">
   <si>
     <t>Estimate</t>
   </si>
@@ -815,6 +820,18 @@
 I can order alphabetically.
 I can order by target date.
 The system can compute the numerical value of each task in relation to that of the overall sprint as a percentage of the total effort required. 
+</t>
+  </si>
+  <si>
+    <t>Subtasks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Set up IDE 
+* Set up PHP framework
+* Create database table for called Users
+* Create registration form
+* Create query to add user information to the database table
+* Form input validation 
 </t>
   </si>
 </sst>
@@ -1291,26 +1308,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="64.42578125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" style="11" customWidth="1"/>
-    <col min="7" max="256" width="25.42578125" style="10" customWidth="1"/>
-    <col min="257" max="16384" width="9.140625" style="10"/>
+    <col min="1" max="1" width="16.5" style="12" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="55.1640625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="64.5" style="10" customWidth="1"/>
+    <col min="7" max="7" width="25.5" style="11" customWidth="1"/>
+    <col min="8" max="257" width="25.5" style="10" customWidth="1"/>
+    <col min="258" max="16384" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="20" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="20" customFormat="1" ht="22.5" customHeight="1">
       <c r="A1" s="23" t="s">
         <v>203</v>
       </c>
@@ -1320,17 +1338,20 @@
       <c r="C1" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="66">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -1340,37 +1361,39 @@
       <c r="C2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="16"/>
+      <c r="E2" s="11">
         <v>10</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="F2" s="11">
+      <c r="G2" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="88">
       <c r="A3" s="12">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="17"/>
+      <c r="E3" s="11">
         <v>10</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="F3" s="11">
+      <c r="G3" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="70">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -1380,17 +1403,18 @@
       <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="16"/>
+      <c r="E4" s="11">
         <v>3</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="F4" s="11">
+      <c r="G4" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="90">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -1400,17 +1424,20 @@
       <c r="C5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="12">
-        <v>3</v>
-      </c>
-      <c r="E5" s="13" t="s">
+      <c r="D5" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5" s="12">
+        <v>7</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="F5" s="12">
+      <c r="G5" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="40">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -1420,17 +1447,18 @@
       <c r="C6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="16"/>
+      <c r="E6" s="11">
         <v>1</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="F6" s="11">
+      <c r="G6" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="60">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -1440,17 +1468,18 @@
       <c r="C7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="16"/>
+      <c r="E7" s="11">
         <v>3</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="F7" s="11">
+      <c r="G7" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="44">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -1460,17 +1489,17 @@
       <c r="C8" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="D8" s="11">
-        <v>5</v>
-      </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="11">
+        <v>5</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="F8" s="11">
+      <c r="G8" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="33">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -1480,17 +1509,18 @@
       <c r="C9" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="16"/>
+      <c r="E9" s="11">
         <v>1</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="F9" s="11">
+      <c r="G9" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="55">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -1500,17 +1530,18 @@
       <c r="C10" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="17"/>
+      <c r="E10" s="11">
         <v>10</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="F10" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="F10" s="11">
+      <c r="G10" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="33">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -1520,17 +1551,17 @@
       <c r="C11" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="D11" s="11">
+      <c r="E11" s="11">
         <v>10</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="F11" s="11">
+      <c r="G11" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="66">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -1540,17 +1571,18 @@
       <c r="C12" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="16"/>
+      <c r="E12" s="11">
         <v>10</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="F12" s="11">
+      <c r="G12" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="33">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -1560,17 +1592,18 @@
       <c r="C13" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="11">
-        <v>5</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="17"/>
+      <c r="E13" s="11">
+        <v>5</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="F13" s="11">
+      <c r="G13" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="44">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -1580,17 +1613,17 @@
       <c r="C14" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="D14" s="11">
+      <c r="E14" s="11">
         <v>1</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="F14" s="11">
+      <c r="G14" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="44">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -1600,17 +1633,17 @@
       <c r="C15" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="11">
+      <c r="E15" s="11">
         <v>3</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="F15" s="11">
+      <c r="G15" s="11">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="55">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -1620,17 +1653,17 @@
       <c r="C16" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D16" s="11">
-        <v>5</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="11">
+        <v>5</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="F16" s="11">
+      <c r="G16" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="33">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -1640,17 +1673,18 @@
       <c r="C17" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="18"/>
+      <c r="E17" s="11">
         <v>10</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="F17" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="F17" s="11">
+      <c r="G17" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="33">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -1660,17 +1694,17 @@
       <c r="C18" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="11">
+      <c r="E18" s="11">
         <v>10</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="F18" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="G18" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="44">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -1680,17 +1714,17 @@
       <c r="C19" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="D19" s="11">
+      <c r="E19" s="11">
         <v>10</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="F19" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F19" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="G19" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="33">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -1700,17 +1734,17 @@
       <c r="C20" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="11">
+      <c r="E20" s="11">
         <v>3</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="F20" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="F20" s="11">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="G20" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="22">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -1720,17 +1754,17 @@
       <c r="C21" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D21" s="11">
-        <v>5</v>
-      </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="11">
+        <v>5</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="33">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -1740,17 +1774,17 @@
       <c r="C22" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="D22" s="11">
-        <v>5</v>
-      </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="11">
+        <v>5</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="G22" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="44">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -1760,17 +1794,18 @@
       <c r="C23" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="19"/>
+      <c r="E23" s="11">
         <v>10</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="F23" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="22">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -1780,17 +1815,17 @@
       <c r="C24" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="D24" s="11">
+      <c r="E24" s="11">
         <v>10</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="66">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -1800,17 +1835,17 @@
       <c r="C25" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="11">
+      <c r="E25" s="11">
         <v>20</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="F25" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="44">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -1820,17 +1855,17 @@
       <c r="C26" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="D26" s="11">
+      <c r="E26" s="11">
         <v>20</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="F26" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="G26" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="44">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -1840,17 +1875,18 @@
       <c r="C27" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="18"/>
+      <c r="E27" s="11">
         <v>10</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="F27" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="33">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -1860,19 +1896,24 @@
       <c r="C28" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="D28" s="11">
+      <c r="E28" s="11">
         <v>20</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="F28" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="G28" s="11" t="s">
         <v>204</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1884,845 +1925,850 @@
       <selection activeCell="A7" sqref="A7:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="17">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1">
       <c r="A38" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1">
       <c r="A42" s="7" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" ht="17">
       <c r="A45" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1">
       <c r="A59" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1">
       <c r="A60" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1">
       <c r="A61" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1">
       <c r="A62" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1">
       <c r="A63" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1">
       <c r="A64" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1">
       <c r="A66" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1">
       <c r="A67" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1">
       <c r="A68" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1">
       <c r="A69" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1">
       <c r="A70" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1">
       <c r="A71" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1">
       <c r="A72" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1">
       <c r="A73" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1">
       <c r="A75" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" ht="17">
       <c r="A78" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1">
       <c r="A80" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1">
       <c r="A81" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1">
       <c r="A82" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1">
       <c r="A83" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1">
       <c r="A84" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1">
       <c r="A85" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1">
       <c r="A86" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1">
       <c r="A87" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1">
       <c r="A88" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1">
       <c r="A89" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1">
       <c r="A90" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1">
       <c r="A91" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1">
       <c r="A93" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1">
       <c r="A94" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1">
       <c r="A95" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1">
       <c r="A96" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1">
       <c r="A97" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1">
       <c r="A99" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1">
       <c r="A100" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1">
       <c r="A101" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1">
       <c r="A102" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1">
       <c r="A103" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1">
       <c r="A104" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1">
       <c r="A105" s="3"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1">
       <c r="A106" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" ht="17">
       <c r="A109" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1">
       <c r="A111" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1">
       <c r="A112" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1">
       <c r="A113" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1">
       <c r="A114" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1">
       <c r="A115" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1">
       <c r="A116" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1">
       <c r="A117" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1">
       <c r="A118" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1">
       <c r="A119" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1">
       <c r="A120" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1">
       <c r="A121" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1">
       <c r="A122" s="3"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1">
       <c r="A123" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1">
       <c r="A124" s="5" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1">
       <c r="A125" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1">
       <c r="A126" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1">
       <c r="A127" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1">
       <c r="A129" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" ht="17">
       <c r="A132" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1">
       <c r="A134" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1">
       <c r="A135" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1">
       <c r="A136" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1">
       <c r="A137" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1">
       <c r="A138" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1">
       <c r="A139" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1">
       <c r="A140" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1">
       <c r="A141" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1">
       <c r="A142" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1">
       <c r="A143" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1">
       <c r="A145" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1">
       <c r="A146" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1">
       <c r="A147" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1">
       <c r="A148" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" ht="17">
       <c r="A151" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1">
       <c r="A153" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1">
       <c r="A154" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1">
       <c r="A155" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1">
       <c r="A156" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1">
       <c r="A157" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1">
       <c r="A158" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1">
       <c r="A159" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1">
       <c r="A160" s="6" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1">
       <c r="A161" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1">
       <c r="A162" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1">
       <c r="A163" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1">
       <c r="A164" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1">
       <c r="A165" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1">
       <c r="A166" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1">
       <c r="A167" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1">
       <c r="A168" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1">
       <c r="A169" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1">
       <c r="A170" s="3"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:1">
       <c r="A171" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:1">
       <c r="A172" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:1">
       <c r="A173" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:1">
       <c r="A174" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:1">
       <c r="A175" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:1">
       <c r="A176" s="4" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:1">
       <c r="A177" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:1">
       <c r="A178" s="5" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:1">
       <c r="A179" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:1">
       <c r="A180" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:1">
       <c r="A181" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:1">
       <c r="A182" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:1">
       <c r="A183" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:1">
       <c r="A184" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:1">
       <c r="A185" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:1">
       <c r="A186" s="3"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:1">
       <c r="A187" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:1">
       <c r="A188" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:1">
       <c r="A189" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:1">
       <c r="A190" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:1">
       <c r="A191" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:1">
       <c r="A192" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:1">
       <c r="A193" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:1">
       <c r="A194" s="5" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:1">
       <c r="A195" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:1">
       <c r="A196" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:1">
       <c r="A197" s="4" t="s">
         <v>141</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>